<commit_message>
urb_area_id_preg added in non rep data dictionary
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_5/1_5_non_rep.xlsx
+++ b/dictionaries/urban_ath/1_5/1_5_non_rep.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demetrisavraam/Desktop/GitHub/ds-dictionaries/dictionaries/urban_ath/1_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6185AEAB-4511-F644-8BFF-5E31967E4ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D8B937-F9B0-7948-AF8C-60458E787DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20880" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Categories!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$218</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$219</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="550">
   <si>
     <t>name</t>
   </si>
@@ -1673,7 +1673,13 @@
     <t>urb_area_id_0</t>
   </si>
   <si>
-    <t xml:space="preserve">unique identifier for the urban area (for the cohorts with children moving from one area to another at different time periods) </t>
+    <t>urb_area_id_preg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique identifier for the urban area at pregnancy (for the cohorts with children moving from one area to another at different time periods) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique identifier for the urban area at birth (for the cohorts with children moving from one area to another at different time periods) </t>
   </si>
 </sst>
 </file>
@@ -2581,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMH219"/>
+  <dimension ref="A1:AMH220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:XFD104"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10131,26 +10137,24 @@
       </c>
       <c r="C104"/>
       <c r="D104" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>232</v>
+        <v>547</v>
       </c>
       <c r="B105" t="s">
-        <v>18</v>
-      </c>
-      <c r="C105" t="s">
-        <v>19</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C105"/>
       <c r="D105" t="s">
-        <v>233</v>
+        <v>548</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B106" t="s">
         <v>18</v>
@@ -10159,50 +10163,50 @@
         <v>19</v>
       </c>
       <c r="D106" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107"/>
+        <v>18</v>
+      </c>
+      <c r="C107" t="s">
+        <v>19</v>
+      </c>
       <c r="D107" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B108" t="s">
         <v>5</v>
       </c>
       <c r="C108"/>
       <c r="D108" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B109" t="s">
-        <v>18</v>
-      </c>
-      <c r="C109" t="s">
-        <v>28</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C109"/>
       <c r="D109" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B110" t="s">
         <v>18</v>
@@ -10211,66 +10215,66 @@
         <v>28</v>
       </c>
       <c r="D110" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B111" t="s">
         <v>18</v>
       </c>
       <c r="C111" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D111" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B112" t="s">
         <v>18</v>
       </c>
       <c r="C112" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D112" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113"/>
+        <v>18</v>
+      </c>
+      <c r="C113" t="s">
+        <v>36</v>
+      </c>
       <c r="D113" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B114" t="s">
-        <v>18</v>
-      </c>
-      <c r="C114" t="s">
-        <v>41</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C114"/>
       <c r="D114" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B115" t="s">
         <v>18</v>
@@ -10279,40 +10283,40 @@
         <v>41</v>
       </c>
       <c r="D115" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B116" t="s">
         <v>18</v>
       </c>
       <c r="C116" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D116" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B117" t="s">
         <v>18</v>
       </c>
       <c r="C117" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D117" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>458</v>
+        <v>256</v>
       </c>
       <c r="B118" t="s">
         <v>18</v>
@@ -10321,12 +10325,12 @@
         <v>41</v>
       </c>
       <c r="D118" t="s">
-        <v>502</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B119" t="s">
         <v>18</v>
@@ -10335,12 +10339,12 @@
         <v>41</v>
       </c>
       <c r="D119" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B120" t="s">
         <v>18</v>
@@ -10349,12 +10353,12 @@
         <v>41</v>
       </c>
       <c r="D120" t="s">
-        <v>504</v>
+        <v>522</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B121" t="s">
         <v>18</v>
@@ -10363,12 +10367,12 @@
         <v>41</v>
       </c>
       <c r="D121" t="s">
-        <v>539</v>
+        <v>504</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B122" t="s">
         <v>18</v>
@@ -10377,12 +10381,12 @@
         <v>41</v>
       </c>
       <c r="D122" t="s">
-        <v>505</v>
+        <v>539</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B123" t="s">
         <v>18</v>
@@ -10391,12 +10395,12 @@
         <v>41</v>
       </c>
       <c r="D123" t="s">
-        <v>524</v>
+        <v>505</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B124" t="s">
         <v>18</v>
@@ -10405,12 +10409,12 @@
         <v>41</v>
       </c>
       <c r="D124" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B125" t="s">
         <v>18</v>
@@ -10419,12 +10423,12 @@
         <v>41</v>
       </c>
       <c r="D125" t="s">
-        <v>525</v>
+        <v>506</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B126" t="s">
         <v>18</v>
@@ -10433,12 +10437,12 @@
         <v>41</v>
       </c>
       <c r="D126" t="s">
-        <v>507</v>
+        <v>525</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B127" t="s">
         <v>18</v>
@@ -10447,12 +10451,12 @@
         <v>41</v>
       </c>
       <c r="D127" t="s">
-        <v>526</v>
+        <v>507</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B128" t="s">
         <v>18</v>
@@ -10461,12 +10465,12 @@
         <v>41</v>
       </c>
       <c r="D128" t="s">
-        <v>508</v>
+        <v>526</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B129" t="s">
         <v>18</v>
@@ -10475,12 +10479,12 @@
         <v>41</v>
       </c>
       <c r="D129" t="s">
-        <v>527</v>
+        <v>508</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B130" t="s">
         <v>18</v>
@@ -10489,12 +10493,12 @@
         <v>41</v>
       </c>
       <c r="D130" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B131" t="s">
         <v>18</v>
@@ -10503,12 +10507,12 @@
         <v>41</v>
       </c>
       <c r="D131" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B132" t="s">
         <v>18</v>
@@ -10517,12 +10521,12 @@
         <v>41</v>
       </c>
       <c r="D132" t="s">
-        <v>514</v>
+        <v>528</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B133" t="s">
         <v>18</v>
@@ -10531,12 +10535,12 @@
         <v>41</v>
       </c>
       <c r="D133" t="s">
-        <v>541</v>
+        <v>514</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B134" t="s">
         <v>18</v>
@@ -10545,12 +10549,12 @@
         <v>41</v>
       </c>
       <c r="D134" t="s">
-        <v>509</v>
+        <v>541</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B135" t="s">
         <v>18</v>
@@ -10559,12 +10563,12 @@
         <v>41</v>
       </c>
       <c r="D135" t="s">
-        <v>542</v>
+        <v>509</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B136" t="s">
         <v>18</v>
@@ -10573,12 +10577,12 @@
         <v>41</v>
       </c>
       <c r="D136" t="s">
-        <v>510</v>
+        <v>542</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B137" t="s">
         <v>18</v>
@@ -10587,12 +10591,12 @@
         <v>41</v>
       </c>
       <c r="D137" t="s">
-        <v>543</v>
+        <v>510</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B138" t="s">
         <v>18</v>
@@ -10601,12 +10605,12 @@
         <v>41</v>
       </c>
       <c r="D138" t="s">
-        <v>511</v>
+        <v>543</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B139" t="s">
         <v>18</v>
@@ -10615,12 +10619,12 @@
         <v>41</v>
       </c>
       <c r="D139" t="s">
-        <v>544</v>
+        <v>511</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B140" t="s">
         <v>18</v>
@@ -10629,12 +10633,12 @@
         <v>41</v>
       </c>
       <c r="D140" t="s">
-        <v>503</v>
+        <v>544</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B141" t="s">
         <v>18</v>
@@ -10643,12 +10647,12 @@
         <v>41</v>
       </c>
       <c r="D141" t="s">
-        <v>533</v>
+        <v>503</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B142" t="s">
         <v>18</v>
@@ -10657,12 +10661,12 @@
         <v>41</v>
       </c>
       <c r="D142" t="s">
-        <v>512</v>
+        <v>533</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B143" t="s">
         <v>18</v>
@@ -10671,12 +10675,12 @@
         <v>41</v>
       </c>
       <c r="D143" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B144" t="s">
         <v>18</v>
@@ -10685,12 +10689,12 @@
         <v>41</v>
       </c>
       <c r="D144" t="s">
-        <v>513</v>
+        <v>523</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B145" t="s">
         <v>18</v>
@@ -10699,12 +10703,12 @@
         <v>41</v>
       </c>
       <c r="D145" t="s">
-        <v>534</v>
+        <v>513</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B146" t="s">
         <v>18</v>
@@ -10713,12 +10717,12 @@
         <v>41</v>
       </c>
       <c r="D146" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B147" t="s">
         <v>18</v>
@@ -10727,12 +10731,12 @@
         <v>41</v>
       </c>
       <c r="D147" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B148" t="s">
         <v>18</v>
@@ -10741,12 +10745,12 @@
         <v>41</v>
       </c>
       <c r="D148" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B149" t="s">
         <v>18</v>
@@ -10755,12 +10759,12 @@
         <v>41</v>
       </c>
       <c r="D149" t="s">
-        <v>536</v>
+        <v>515</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B150" t="s">
         <v>18</v>
@@ -10769,12 +10773,12 @@
         <v>41</v>
       </c>
       <c r="D150" t="s">
-        <v>516</v>
+        <v>536</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B151" t="s">
         <v>18</v>
@@ -10783,12 +10787,12 @@
         <v>41</v>
       </c>
       <c r="D151" t="s">
-        <v>537</v>
+        <v>516</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B152" t="s">
         <v>18</v>
@@ -10797,12 +10801,12 @@
         <v>41</v>
       </c>
       <c r="D152" t="s">
-        <v>517</v>
+        <v>537</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B153" t="s">
         <v>18</v>
@@ -10811,12 +10815,12 @@
         <v>41</v>
       </c>
       <c r="D153" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B154" t="s">
         <v>18</v>
@@ -10825,12 +10829,12 @@
         <v>41</v>
       </c>
       <c r="D154" t="s">
-        <v>518</v>
+        <v>538</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B155" t="s">
         <v>18</v>
@@ -10839,12 +10843,12 @@
         <v>41</v>
       </c>
       <c r="D155" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B156" t="s">
         <v>18</v>
@@ -10853,12 +10857,12 @@
         <v>41</v>
       </c>
       <c r="D156" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B157" t="s">
         <v>18</v>
@@ -10867,12 +10871,12 @@
         <v>41</v>
       </c>
       <c r="D157" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B158" t="s">
         <v>18</v>
@@ -10881,12 +10885,12 @@
         <v>41</v>
       </c>
       <c r="D158" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B159" t="s">
         <v>18</v>
@@ -10895,12 +10899,12 @@
         <v>41</v>
       </c>
       <c r="D159" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B160" t="s">
         <v>18</v>
@@ -10909,12 +10913,12 @@
         <v>41</v>
       </c>
       <c r="D160" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B161" t="s">
         <v>18</v>
@@ -10923,78 +10927,78 @@
         <v>41</v>
       </c>
       <c r="D161" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" t="s">
-        <v>258</v>
+        <v>501</v>
       </c>
       <c r="B162" t="s">
         <v>18</v>
       </c>
-      <c r="C162"/>
+      <c r="C162" t="s">
+        <v>41</v>
+      </c>
       <c r="D162" t="s">
-        <v>259</v>
+        <v>532</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B163" t="s">
         <v>18</v>
       </c>
-      <c r="C163" t="s">
-        <v>33</v>
-      </c>
+      <c r="C163"/>
       <c r="D163" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B164" t="s">
         <v>18</v>
       </c>
       <c r="C164" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D164" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
-      </c>
-      <c r="C165"/>
+        <v>18</v>
+      </c>
+      <c r="C165" t="s">
+        <v>36</v>
+      </c>
       <c r="D165" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B166" t="s">
-        <v>18</v>
-      </c>
-      <c r="C166" t="s">
-        <v>19</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C166"/>
       <c r="D166" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B167" t="s">
         <v>18</v>
@@ -11003,92 +11007,92 @@
         <v>19</v>
       </c>
       <c r="D167" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B168" t="s">
         <v>18</v>
       </c>
       <c r="C168" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="D168" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B169" t="s">
         <v>18</v>
       </c>
-      <c r="C169"/>
+      <c r="C169" t="s">
+        <v>71</v>
+      </c>
       <c r="D169" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C170"/>
       <c r="D170" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B171" t="s">
-        <v>18</v>
-      </c>
-      <c r="C171" t="s">
-        <v>78</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C171"/>
       <c r="D171" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B172" t="s">
         <v>18</v>
       </c>
       <c r="C172" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D172" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B173" t="s">
         <v>18</v>
       </c>
       <c r="C173" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="D173" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B174" t="s">
         <v>18</v>
@@ -11097,12 +11101,12 @@
         <v>83</v>
       </c>
       <c r="D174" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B175" t="s">
         <v>18</v>
@@ -11111,66 +11115,66 @@
         <v>83</v>
       </c>
       <c r="D175" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
-      </c>
-      <c r="C176"/>
+        <v>18</v>
+      </c>
+      <c r="C176" t="s">
+        <v>83</v>
+      </c>
       <c r="D176" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B177" t="s">
-        <v>18</v>
-      </c>
-      <c r="C177" t="s">
-        <v>78</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C177"/>
       <c r="D177" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B178" t="s">
         <v>18</v>
       </c>
       <c r="C178" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D178" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B179" t="s">
         <v>18</v>
       </c>
       <c r="C179" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="D179" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B180" t="s">
         <v>18</v>
@@ -11179,12 +11183,12 @@
         <v>101</v>
       </c>
       <c r="D180" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B181" t="s">
         <v>18</v>
@@ -11193,12 +11197,12 @@
         <v>101</v>
       </c>
       <c r="D181" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B182" t="s">
         <v>18</v>
@@ -11207,12 +11211,12 @@
         <v>101</v>
       </c>
       <c r="D182" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B183" t="s">
         <v>18</v>
@@ -11221,12 +11225,12 @@
         <v>101</v>
       </c>
       <c r="D183" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B184" t="s">
         <v>18</v>
@@ -11235,54 +11239,54 @@
         <v>101</v>
       </c>
       <c r="D184" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B185" t="s">
         <v>18</v>
       </c>
       <c r="C185" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="D185" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B186" t="s">
         <v>18</v>
       </c>
       <c r="C186" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D186" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B187" t="s">
         <v>18</v>
       </c>
       <c r="C187" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="D187" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B188" t="s">
         <v>18</v>
@@ -11291,12 +11295,12 @@
         <v>127</v>
       </c>
       <c r="D188" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B189" t="s">
         <v>18</v>
@@ -11305,12 +11309,12 @@
         <v>127</v>
       </c>
       <c r="D189" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B190" t="s">
         <v>18</v>
@@ -11319,12 +11323,12 @@
         <v>127</v>
       </c>
       <c r="D190" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B191" t="s">
         <v>18</v>
@@ -11333,12 +11337,12 @@
         <v>127</v>
       </c>
       <c r="D191" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B192" t="s">
         <v>18</v>
@@ -11347,12 +11351,12 @@
         <v>127</v>
       </c>
       <c r="D192" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B193" t="s">
         <v>18</v>
@@ -11361,12 +11365,12 @@
         <v>127</v>
       </c>
       <c r="D193" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B194" t="s">
         <v>18</v>
@@ -11375,12 +11379,12 @@
         <v>127</v>
       </c>
       <c r="D194" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B195" t="s">
         <v>18</v>
@@ -11389,12 +11393,12 @@
         <v>127</v>
       </c>
       <c r="D195" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B196" t="s">
         <v>18</v>
@@ -11403,12 +11407,12 @@
         <v>127</v>
       </c>
       <c r="D196" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B197" t="s">
         <v>18</v>
@@ -11417,12 +11421,12 @@
         <v>127</v>
       </c>
       <c r="D197" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A198" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B198" t="s">
         <v>18</v>
@@ -11431,12 +11435,12 @@
         <v>127</v>
       </c>
       <c r="D198" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B199" t="s">
         <v>18</v>
@@ -11445,12 +11449,12 @@
         <v>127</v>
       </c>
       <c r="D199" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B200" t="s">
         <v>18</v>
@@ -11459,12 +11463,12 @@
         <v>127</v>
       </c>
       <c r="D200" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B201" t="s">
         <v>18</v>
@@ -11473,12 +11477,12 @@
         <v>127</v>
       </c>
       <c r="D201" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B202" t="s">
         <v>18</v>
@@ -11487,26 +11491,26 @@
         <v>127</v>
       </c>
       <c r="D202" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B203" t="s">
         <v>18</v>
       </c>
       <c r="C203" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="D203" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B204" t="s">
         <v>18</v>
@@ -11515,40 +11519,40 @@
         <v>19</v>
       </c>
       <c r="D204" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B205" t="s">
         <v>18</v>
       </c>
-      <c r="C205" s="5" t="s">
-        <v>345</v>
+      <c r="C205" t="s">
+        <v>19</v>
       </c>
       <c r="D205" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B206" t="s">
         <v>18</v>
       </c>
-      <c r="C206" t="s">
-        <v>19</v>
+      <c r="C206" s="5" t="s">
+        <v>345</v>
       </c>
       <c r="D206" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B207" t="s">
         <v>18</v>
@@ -11557,26 +11561,26 @@
         <v>19</v>
       </c>
       <c r="D207" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B208" t="s">
         <v>18</v>
       </c>
       <c r="C208" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D208" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B209" t="s">
         <v>18</v>
@@ -11585,12 +11589,12 @@
         <v>41</v>
       </c>
       <c r="D209" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B210" t="s">
         <v>18</v>
@@ -11599,26 +11603,26 @@
         <v>41</v>
       </c>
       <c r="D210" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B211" t="s">
         <v>18</v>
       </c>
-      <c r="C211" s="5" t="s">
-        <v>205</v>
+      <c r="C211" t="s">
+        <v>41</v>
       </c>
       <c r="D211" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B212" t="s">
         <v>18</v>
@@ -11627,40 +11631,40 @@
         <v>205</v>
       </c>
       <c r="D212" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B213" t="s">
         <v>18</v>
       </c>
       <c r="C213" s="5" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="D213" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B214" t="s">
         <v>18</v>
       </c>
-      <c r="C214" t="s">
-        <v>19</v>
+      <c r="C214" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="D214" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B215" t="s">
         <v>18</v>
@@ -11669,12 +11673,12 @@
         <v>19</v>
       </c>
       <c r="D215" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B216" t="s">
         <v>18</v>
@@ -11683,42 +11687,56 @@
         <v>19</v>
       </c>
       <c r="D216" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B217" t="s">
         <v>18</v>
       </c>
-      <c r="C217"/>
+      <c r="C217" t="s">
+        <v>19</v>
+      </c>
       <c r="D217" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" t="s">
+        <v>369</v>
+      </c>
+      <c r="B218" t="s">
+        <v>18</v>
+      </c>
+      <c r="C218"/>
+      <c r="D218" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A219" t="s">
         <v>371</v>
       </c>
-      <c r="B218" t="s">
-        <v>18</v>
-      </c>
-      <c r="C218" t="s">
+      <c r="B219" t="s">
+        <v>18</v>
+      </c>
+      <c r="C219" t="s">
         <v>19</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D219" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C219"/>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C220"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D218" xr:uid="{CB884253-6560-4D16-8383-8D9DA571A935}"/>
+  <autoFilter ref="A1:D219" xr:uid="{CB884253-6560-4D16-8383-8D9DA571A935}"/>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" sqref="B3:B658" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showErrorMessage="1" sqref="B3:B659" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"integer,decimal,text,binary,locale,boolean,datetime,date"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11730,10 +11748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:E188"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12837,80 +12855,80 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>25</v>
+        <v>547</v>
       </c>
       <c r="B79">
-        <v>1</v>
-      </c>
-      <c r="C79" s="6" t="b">
+        <v>1401</v>
+      </c>
+      <c r="C79" t="b">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>25</v>
+        <v>547</v>
       </c>
       <c r="B80">
-        <v>2</v>
-      </c>
-      <c r="C80" s="6" t="b">
+        <v>1402</v>
+      </c>
+      <c r="C80" t="b">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>25</v>
+        <v>547</v>
       </c>
       <c r="B81">
-        <v>3</v>
-      </c>
-      <c r="C81" s="6" t="b">
+        <v>1403</v>
+      </c>
+      <c r="C81" t="b">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>547</v>
       </c>
       <c r="B82">
-        <v>1</v>
-      </c>
-      <c r="C82" s="6" t="b">
+        <v>1404</v>
+      </c>
+      <c r="C82" t="b">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C83" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84" s="6" t="b">
         <v>0</v>
@@ -12921,16 +12939,16 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C85" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
@@ -12938,69 +12956,69 @@
         <v>23</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C86" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C87" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C88" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C89" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
@@ -13008,13 +13026,13 @@
         <v>75</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C91" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
@@ -13022,69 +13040,69 @@
         <v>75</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C92" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C93" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B94">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C94" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B95">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C95" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B96">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C96" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
@@ -13092,13 +13110,13 @@
         <v>89</v>
       </c>
       <c r="B97">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C97" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
@@ -13106,74 +13124,74 @@
         <v>89</v>
       </c>
       <c r="B98">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C98" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C99" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>238</v>
+        <v>89</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C100" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>238</v>
+        <v>89</v>
       </c>
       <c r="B101">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C101" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>238</v>
+        <v>89</v>
       </c>
       <c r="B102">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C102" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>236</v>
+        <v>56</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -13182,29 +13200,29 @@
         <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C104" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C105" s="6" t="b">
         <v>0</v>
@@ -13215,16 +13233,16 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B106">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C106" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
@@ -13232,69 +13250,69 @@
         <v>236</v>
       </c>
       <c r="B107">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C107" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C108" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C109" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C110" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D110" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C111" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D111" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
@@ -13302,13 +13320,13 @@
         <v>274</v>
       </c>
       <c r="B112">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C112" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D112" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
@@ -13316,69 +13334,69 @@
         <v>274</v>
       </c>
       <c r="B113">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C113" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D113" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C114" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D114" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B115">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C115" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D115" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C116" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B117">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C117" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D117" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
@@ -13386,13 +13404,13 @@
         <v>286</v>
       </c>
       <c r="B118">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C118" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D118" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
@@ -13400,76 +13418,76 @@
         <v>286</v>
       </c>
       <c r="B119">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C119" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>248</v>
+        <v>286</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C120" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C121" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D121" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>38</v>
-      </c>
-      <c r="B122" s="1">
-        <v>0</v>
+        <v>286</v>
+      </c>
+      <c r="B122">
+        <v>5</v>
       </c>
       <c r="C122" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D122" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>38</v>
-      </c>
-      <c r="B123" s="1">
-        <v>1</v>
+        <v>286</v>
+      </c>
+      <c r="B123">
+        <v>6</v>
       </c>
       <c r="C123" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D123" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>56</v>
-      </c>
-      <c r="B124" s="1">
+        <v>248</v>
+      </c>
+      <c r="B124">
         <v>0</v>
       </c>
       <c r="C124" s="6" t="b">
@@ -13481,9 +13499,9 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>248</v>
-      </c>
-      <c r="B125" s="1">
+        <v>264</v>
+      </c>
+      <c r="B125">
         <v>1</v>
       </c>
       <c r="C125" s="6" t="b">
@@ -13495,7 +13513,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>264</v>
+        <v>38</v>
       </c>
       <c r="B126" s="1">
         <v>0</v>
@@ -13508,57 +13526,101 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B127" s="1"/>
+      <c r="A127" t="s">
+        <v>38</v>
+      </c>
+      <c r="B127" s="1">
+        <v>1</v>
+      </c>
+      <c r="C127" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D127" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B128" s="1"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B130" s="1"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="A128" t="s">
+        <v>56</v>
+      </c>
+      <c r="B128" s="1">
+        <v>0</v>
+      </c>
+      <c r="C128" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D128" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A129" t="s">
+        <v>248</v>
+      </c>
+      <c r="B129" s="1">
+        <v>1</v>
+      </c>
+      <c r="C129" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D129" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A130" t="s">
+        <v>264</v>
+      </c>
+      <c r="B130" s="1">
+        <v>0</v>
+      </c>
+      <c r="C130" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D130" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B132" s="1"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B133" s="1"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B134" s="1"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B135" s="1"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B136" s="1"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B137" s="1"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B144" s="1"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.15">
@@ -13680,6 +13742,18 @@
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B184" s="1"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B185" s="1"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B186" s="1"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B187" s="1"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B188" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>

</xml_diff>